<commit_message>
added 4l4y script converter
</commit_message>
<xml_diff>
--- a/pretrained_model/sms_classifier_corpus/collected_sms_database/All SMSCollection.xlsx
+++ b/pretrained_model/sms_classifier_corpus/collected_sms_database/All SMSCollection.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8505"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="876">
   <si>
     <t>Jenis SMS</t>
   </si>
@@ -6787,18 +6787,231 @@
   <si>
     <t>BUY 1 GET 1 FREE BERGO ZOYA! Tunjukkan SMS ini di ZOYA Kalimalang Blok 7 No13-14 Hanya berlaku hari ini. S&amp;K Berlaku. Promo*606#</t>
   </si>
+  <si>
+    <t>Mama minta pulsa dong dek, lagi kehabisan nih. Tolong kirim ya ke +62813748293847</t>
+  </si>
+  <si>
+    <t>mama minta pulsa 50rb, kirim ke +62813748293847 mama ada urusan di kantor polisi, mama make hp org lain. thx</t>
+  </si>
+  <si>
+    <t>WOI MAMA MINTA PULSA 50RB ANJINK! CEPETAN!</t>
+  </si>
+  <si>
+    <t>woi emak minta pulsa 50 rebu ke nomer +62813748293847 emak abis malakin orang sekarang ada di kantor polisi, ini make hape hasil palakan</t>
+  </si>
+  <si>
+    <t>mama minta 5 GOLD kirim ke +62813748293847 mama make ID ORG soalnya ID mama lagi error. terimakasih.</t>
+  </si>
+  <si>
+    <t>mama minta pulsa 50rb ke nomer +62813748293847 mama make nomer orang lain, soalnya pulsa mama abis, ga ada duit soalnya kena penipuan berhadiah. thanks.</t>
+  </si>
+  <si>
+    <t>mama minta cash PB 50 rb ke ID +62813748293847 emak mau beli Kriss S.V.D 30 hari tapi cashnya ga cukup. ini emak make ID laen soalnya ID emak lagi dipake adek. makasih.</t>
+  </si>
+  <si>
+    <t>mama minta pulsa 100rb ke nomer +62813748293847 mama make nomer orang lain soalnya pulsa mama abis kena penipuan mama minta pulsa. thanx.</t>
+  </si>
+  <si>
+    <t>sayang, kirimin aku pulsa 300 juta dong ke nomer +62813748293847 ini make BB temenku soalnya pulsa iPhoneku abis.</t>
+  </si>
+  <si>
+    <t>m4M4 mN7 pL54 50rB k nMr +62813748293847 4q mK nMr 0r6 lyN kRn d m5lH d kN7r pL151. tHxZzZzZz,,,,</t>
+  </si>
+  <si>
+    <t>Papa mau minta pulsa dong dek, lagi kehabisan nih. Tolong kirim ya ke +62813748293847</t>
+  </si>
+  <si>
+    <t>papa mau minta pulsa 50rb, kirim ke +62813748293847 mama ada urusan di kantor polisi, mama make hp org lain. thx</t>
+  </si>
+  <si>
+    <t>woi papa mau  minta pulsa 50 rebu ke nomer +62813748293847 emak abis malakin orang sekarang ada di kantor polisi, ini make hape hasil palakan</t>
+  </si>
+  <si>
+    <t>papa mau  minta cash PB 50 rb ke ID +62813748293847 emak mau beli Kriss S.V.D 30 hari tapi cashnya ga cukup. ini emak make ID laen soalnya ID emak lagi dipake adek. makasih.</t>
+  </si>
+  <si>
+    <t>papa mau  minta 5 GOLD kirim ke +62813748293847 mama make ID ORG soalnya ID mama lagi error. terimakasih.</t>
+  </si>
+  <si>
+    <t>papa mau  minta pulsa 100rb ke nomer +62813748293847 mama make nomer orang lain soalnya pulsa mama abis kena penipuan mama minta pulsa. thanx.</t>
+  </si>
+  <si>
+    <t>papa mau  minta pulsa 50rb ke nomer +62813748293847 mama make nomer orang lain, soalnya pulsa mama abis, ga ada duit soalnya kena penipuan berhadiah. thanks.</t>
+  </si>
+  <si>
+    <t>papa sayang, kirimin aku pulsa 300 juta dong ke nomer +62813748293847 ini make BB temenku soalnya pulsa iPhoneku abis.</t>
+  </si>
+  <si>
+    <t>p4P4 mN7 pL54 50rB k nMr +62813748293847 4q mK nMr 0r6 lyN kRn d m5lH d kN7r pL151. tHxZzZzZz,,,,</t>
+  </si>
+  <si>
+    <t>WOI PAPA MINTA PULSA 50RB ANJINK! CEPETAN!</t>
+  </si>
+  <si>
+    <t>sayang beli’in duLu pulsa 10rb, di nmr ini, 082191285937, nanti aq yg tlpn km, ini aq pke hp tmen, skrg yacc!</t>
+  </si>
+  <si>
+    <t>Ini mama pake hp temen, Mama sedang dalam keadaan darurat dan tertimpa musibah, tolong kirim mama pulsa ke no. +62813748293847 Jgn telpon dulu</t>
+  </si>
+  <si>
+    <t>Tolong kirimkan mama pulsa Rp 5 ribu. Mama lagi berurusan dengan polisi. Jadi Jangan dihubung</t>
+  </si>
+  <si>
+    <t>mama… papa lagi dikontor polisi, tolong kirimin pulsa pulsa Rp10.000 Ke no 08XXXXXXXXXX, Ini Papa pakai hp teman, jangan telepon papa lagi sibuk</t>
+  </si>
+  <si>
+    <t>Mau Transfer Pakai Bank Apa, atau Tlp dlu ke no sy yg ini 087820088889: T'ks</t>
+  </si>
+  <si>
+    <t>Dlm program MANDIRI FIESTA, no rek anda mendapatkan cek Rp 75jt kode PIN 777777FD.INFO klik www.info-undianmandiri.blogspot.com</t>
+  </si>
+  <si>
+    <t>gw rapat singkat aja karena dikit yg mau diomongin, abis itu siap2 pasangin manila</t>
+  </si>
+  <si>
+    <t>perlu bikin daftar nama gak?</t>
+  </si>
+  <si>
+    <t>putih dulu aj ya sementara</t>
+  </si>
+  <si>
+    <t>guys maaf mendadak nih, tapi untuk besok ada yg punya kamera untuk dipinjam gak?</t>
+  </si>
+  <si>
+    <t>gw baru inget kita perlu foto untuk ID Card</t>
+  </si>
+  <si>
+    <t>jangan ilang</t>
+  </si>
+  <si>
+    <t>anak KG ada yang punya fd yg bisa dipinjam kah besok ???</t>
+  </si>
+  <si>
+    <t>pythonnya udh bisa convert alay yah</t>
+  </si>
+  <si>
+    <t>Palingan minta tolong filter no telp deh</t>
+  </si>
+  <si>
+    <t>Jd kita anggap dia spam, tapi harusnya bkn</t>
+  </si>
+  <si>
+    <t>Tapi jangan sampai pesan biasa masuk spam</t>
+  </si>
+  <si>
+    <t>Ntar dia cek ke masing" model gitu?</t>
+  </si>
+  <si>
+    <t>Trus tiap model kasih tau pendapat</t>
+  </si>
+  <si>
+    <t>Model yg digenerate jd banyak?</t>
+  </si>
+  <si>
+    <t>Atau gmn?</t>
+  </si>
+  <si>
+    <t>Kenapa org pada ga pakai sih</t>
+  </si>
+  <si>
+    <t>gatau sih, gw sih kepikiran aja tadi</t>
+  </si>
+  <si>
+    <t>Trus lu bikinnya gmn?</t>
+  </si>
+  <si>
+    <t>Org sama sekali blm pernah bikin sistwm voting?</t>
+  </si>
+  <si>
+    <t>Itu ide sendiri atau gmn?</t>
+  </si>
+  <si>
+    <t>Tiap algorithm ngasih tau hasilnya?</t>
+  </si>
+  <si>
+    <t>nanti ada sistem voting untuk menentukan jenis message apa yang paling disetujui oleh algoritma-algoritma yang ada</t>
+  </si>
+  <si>
+    <t>iya setiap algoritma akan melabelkan message menurut trainingnya masing"</t>
+  </si>
+  <si>
+    <t>pake sistem voting untuk tentuin message</t>
+  </si>
+  <si>
+    <t>Kalau banyak nanti gw jelasin semua pusing jug</t>
+  </si>
+  <si>
+    <t>Pastikan bisa jelasin algoritma ai nya ya</t>
+  </si>
+  <si>
+    <t>Biar ga nge break kalau di tengah-tengah sms ada &amp; atau "</t>
+  </si>
+  <si>
+    <t>tapi urlencode dulu sblm dikirim</t>
+  </si>
+  <si>
+    <t>API pake query string dlu gpp ya?</t>
+  </si>
+  <si>
+    <t>Moga bisa</t>
+  </si>
+  <si>
+    <t>Bisa lgsg load? Kalau bs yowes deh gaada splash</t>
+  </si>
+  <si>
+    <t>Lagian harusnya kalau ini sih udah ke load</t>
+  </si>
+  <si>
+    <t>Kan tujuan utamanya mempermudah</t>
+  </si>
+  <si>
+    <t>Mana ada app chatting ada loading</t>
+  </si>
+  <si>
+    <t>Di klik ntar pindah activity</t>
+  </si>
+  <si>
+    <t>Kalau API gw msih bantu deh, soalnya masih perlu diupdate</t>
+  </si>
+  <si>
+    <t>Gw ga tahu menahu lagi ya yg android, gw fokus py aja</t>
+  </si>
+  <si>
+    <t>Gw mau bikin kayak Gmail main activity nya</t>
+  </si>
+  <si>
+    <t>Kalau emg ada yg lbih bagus yowes</t>
+  </si>
+  <si>
+    <t>Lagian gw mau bikin bagus sih</t>
+  </si>
+  <si>
+    <t>Jadi kalau ada sms masuk, tapi ga masuk ke notif sama aja boong</t>
+  </si>
+  <si>
+    <t>Karna concern utama kita itu notifikasi kan</t>
+  </si>
+  <si>
+    <t>Berarti tinggal request permission contacts kan?</t>
+  </si>
+  <si>
+    <t>papa aku lagi di kntr polisi, tolong kirimin pulsa dong ke nomor +6289016453723</t>
+  </si>
+  <si>
+    <t>bu anak ibu masuk rumah sakit nih di daerah tomang tolong trf uang sebanyak 2jt cepat ke rek BCA 646273626163</t>
+  </si>
+  <si>
+    <t>pak aku ketabrak mobil tolong kirmin uang dong ke rek BCA 438347271236 buat biaya rumah sakit pa</t>
+  </si>
+  <si>
+    <t>halo selamat pagi sy pak sugianto dari hansip ingin mmbritahukan bhwa ank ibu sdg menjalanai pmrksaan di kntr sy krn trtangkap brklahi di jalan, tlg ibu kirim uang sbnyk 2 jt untuk mnbus dia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6807,351 +7020,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -7174,260 +7064,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -7436,58 +7084,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -7749,26 +7356,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:P1019"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P1094"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="183.428571428571" customWidth="1"/>
-    <col min="15" max="15" width="12.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="183.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7776,7 +7383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="15.75" spans="1:16">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>0</v>
       </c>
@@ -7790,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" spans="1:16">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>0</v>
       </c>
@@ -7804,7 +7411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" spans="1:16">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>0</v>
       </c>
@@ -7818,7 +7425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" ht="15.75" spans="1:2">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>0</v>
       </c>
@@ -7826,7 +7433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" ht="15.75" spans="1:2">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>0</v>
       </c>
@@ -7834,7 +7441,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="15.75" spans="1:2">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>1</v>
       </c>
@@ -7842,7 +7449,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" ht="15.75" spans="1:2">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>0</v>
       </c>
@@ -7850,7 +7457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" ht="15.75" spans="1:2">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>1</v>
       </c>
@@ -7858,7 +7465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" ht="15.75" spans="1:2">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>0</v>
       </c>
@@ -7866,7 +7473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="15.75" spans="1:2">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>1</v>
       </c>
@@ -7874,7 +7481,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" ht="15.75" spans="1:2">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>1</v>
       </c>
@@ -7882,7 +7489,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" ht="15.75" spans="1:2">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>1</v>
       </c>
@@ -7890,7 +7497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" ht="15.75" spans="1:2">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>0</v>
       </c>
@@ -7898,7 +7505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" ht="15.75" spans="1:2">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>0</v>
       </c>
@@ -7906,7 +7513,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" ht="15.75" spans="1:2">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>0</v>
       </c>
@@ -7914,7 +7521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" ht="15.75" spans="1:2">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -7922,7 +7529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" ht="15.75" spans="1:2">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>0</v>
       </c>
@@ -7930,7 +7537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" ht="15.75" spans="1:2">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>0</v>
       </c>
@@ -7938,7 +7545,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="15.75" spans="1:2">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>0</v>
       </c>
@@ -7946,7 +7553,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" ht="15.75" spans="1:2">
+    <row r="21" spans="1:2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -7954,7 +7561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" ht="15.75" spans="1:2">
+    <row r="22" spans="1:2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -7962,7 +7569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" ht="15.75" spans="1:2">
+    <row r="23" spans="1:2">
       <c r="A23">
         <v>0</v>
       </c>
@@ -7970,7 +7577,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" ht="15.75" spans="1:2">
+    <row r="24" spans="1:2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -7978,7 +7585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" ht="15.75" spans="1:2">
+    <row r="25" spans="1:2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -7986,7 +7593,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" ht="15.75" spans="1:2">
+    <row r="26" spans="1:2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -7994,7 +7601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" ht="15.75" spans="1:2">
+    <row r="27" spans="1:2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -8002,7 +7609,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" ht="15.75" spans="1:2">
+    <row r="28" spans="1:2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -8010,7 +7617,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" ht="15.75" spans="1:2">
+    <row r="29" spans="1:2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -8018,7 +7625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="1:2">
+    <row r="30" spans="1:2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -8026,7 +7633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" ht="15.75" spans="1:2">
+    <row r="31" spans="1:2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -8034,7 +7641,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" ht="15.75" spans="1:2">
+    <row r="32" spans="1:2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -8042,7 +7649,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" ht="15.75" spans="1:2">
+    <row r="33" spans="1:2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -8050,7 +7657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" ht="15.75" spans="1:2">
+    <row r="34" spans="1:2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -8058,7 +7665,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" ht="15.75" spans="1:2">
+    <row r="35" spans="1:2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -8066,7 +7673,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" ht="15.75" spans="1:2">
+    <row r="36" spans="1:2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -8074,7 +7681,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" ht="15.75" spans="1:2">
+    <row r="37" spans="1:2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -8082,7 +7689,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" ht="15.75" spans="1:2">
+    <row r="38" spans="1:2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -8090,7 +7697,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" ht="15.75" spans="1:2">
+    <row r="39" spans="1:2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -8098,7 +7705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" ht="15.75" spans="1:2">
+    <row r="40" spans="1:2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -8106,7 +7713,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" ht="15.75" spans="1:2">
+    <row r="41" spans="1:2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -8114,7 +7721,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" ht="15.75" spans="1:2">
+    <row r="42" spans="1:2">
       <c r="A42">
         <v>0</v>
       </c>
@@ -8122,7 +7729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" ht="15.75" spans="1:2">
+    <row r="43" spans="1:2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -8130,7 +7737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" ht="15.75" spans="1:2">
+    <row r="44" spans="1:2">
       <c r="A44">
         <v>0</v>
       </c>
@@ -8138,7 +7745,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" ht="15.75" spans="1:2">
+    <row r="45" spans="1:2">
       <c r="A45">
         <v>0</v>
       </c>
@@ -8146,7 +7753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" ht="15.75" spans="1:2">
+    <row r="46" spans="1:2">
       <c r="A46">
         <v>0</v>
       </c>
@@ -8154,7 +7761,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" ht="15.75" spans="1:2">
+    <row r="47" spans="1:2">
       <c r="A47">
         <v>0</v>
       </c>
@@ -8162,7 +7769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" ht="15.75" spans="1:2">
+    <row r="48" spans="1:2">
       <c r="A48">
         <v>0</v>
       </c>
@@ -8170,7 +7777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" ht="15.75" spans="1:2">
+    <row r="49" spans="1:2">
       <c r="A49">
         <v>0</v>
       </c>
@@ -8178,7 +7785,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" ht="15.75" spans="1:2">
+    <row r="50" spans="1:2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -8186,7 +7793,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" ht="15.75" spans="1:2">
+    <row r="51" spans="1:2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -8194,7 +7801,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" ht="15.75" spans="1:2">
+    <row r="52" spans="1:2">
       <c r="A52">
         <v>0</v>
       </c>
@@ -8202,7 +7809,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" ht="15.75" spans="1:2">
+    <row r="53" spans="1:2">
       <c r="A53">
         <v>0</v>
       </c>
@@ -8210,7 +7817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" ht="26.25" spans="1:2">
+    <row r="54" spans="1:2">
       <c r="A54">
         <v>0</v>
       </c>
@@ -8218,7 +7825,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="55" ht="15.75" spans="1:2">
+    <row r="55" spans="1:2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -8226,7 +7833,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="56" ht="15.75" spans="1:2">
+    <row r="56" spans="1:2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -8234,7 +7841,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="57" ht="15.75" spans="1:2">
+    <row r="57" spans="1:2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -8242,7 +7849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" ht="15.75" spans="1:2">
+    <row r="58" spans="1:2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -8250,7 +7857,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" ht="15.75" spans="1:2">
+    <row r="59" spans="1:2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -8258,7 +7865,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" ht="15.75" spans="1:2">
+    <row r="60" spans="1:2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -8266,7 +7873,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" ht="15.75" spans="1:2">
+    <row r="61" spans="1:2">
       <c r="A61">
         <v>0</v>
       </c>
@@ -8274,7 +7881,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" ht="15.75" spans="1:2">
+    <row r="62" spans="1:2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -8282,7 +7889,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" ht="15.75" spans="1:2">
+    <row r="63" spans="1:2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -8290,7 +7897,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="64" ht="15.75" spans="1:2">
+    <row r="64" spans="1:2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -8298,7 +7905,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" ht="15.75" spans="1:2">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -8306,7 +7913,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" ht="15.75" spans="1:2">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -8314,7 +7921,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" ht="15.75" spans="1:2">
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>1</v>
       </c>
@@ -8322,7 +7929,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="68" ht="15.75" spans="1:2">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -8330,7 +7937,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" ht="15.75" spans="1:2">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>0</v>
       </c>
@@ -8338,7 +7945,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" ht="15.75" spans="1:2">
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -8346,7 +7953,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" ht="15.75" spans="1:2">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>2</v>
       </c>
@@ -8354,7 +7961,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="72" ht="15.75" spans="1:2">
+    <row r="72" spans="1:2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -8362,7 +7969,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="73" ht="15.75" spans="1:2">
+    <row r="73" spans="1:2">
       <c r="A73">
         <v>0</v>
       </c>
@@ -8370,7 +7977,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="74" ht="15.75" spans="1:2">
+    <row r="74" spans="1:2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -8378,7 +7985,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" ht="15.75" spans="1:2">
+    <row r="75" spans="1:2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -8386,7 +7993,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" ht="15.75" spans="1:2">
+    <row r="76" spans="1:2">
       <c r="A76">
         <v>2</v>
       </c>
@@ -8394,7 +8001,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="77" ht="15.75" spans="1:2">
+    <row r="77" spans="1:2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -8402,7 +8009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="78" ht="15.75" spans="1:2">
+    <row r="78" spans="1:2">
       <c r="A78">
         <v>2</v>
       </c>
@@ -8410,7 +8017,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" ht="15.75" spans="1:2">
+    <row r="79" spans="1:2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -8418,7 +8025,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" ht="15.75" spans="1:2">
+    <row r="80" spans="1:2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -8426,7 +8033,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="81" ht="15.75" spans="1:2">
+    <row r="81" spans="1:2">
       <c r="A81">
         <v>0</v>
       </c>
@@ -8434,7 +8041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="82" ht="15.75" spans="1:2">
+    <row r="82" spans="1:2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -8442,7 +8049,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="83" ht="15.75" spans="1:2">
+    <row r="83" spans="1:2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -8450,7 +8057,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="84" ht="15.75" spans="1:2">
+    <row r="84" spans="1:2">
       <c r="A84">
         <v>0</v>
       </c>
@@ -8458,7 +8065,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" ht="15.75" spans="1:2">
+    <row r="85" spans="1:2">
       <c r="A85">
         <v>2</v>
       </c>
@@ -8466,7 +8073,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" ht="15.75" spans="1:2">
+    <row r="86" spans="1:2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -8474,7 +8081,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="87" ht="15.75" spans="1:2">
+    <row r="87" spans="1:2">
       <c r="A87">
         <v>2</v>
       </c>
@@ -8482,7 +8089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="88" ht="15.75" spans="1:2">
+    <row r="88" spans="1:2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -8490,7 +8097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="89" ht="15.75" spans="1:2">
+    <row r="89" spans="1:2">
       <c r="A89">
         <v>2</v>
       </c>
@@ -8498,7 +8105,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="90" ht="15.75" spans="1:2">
+    <row r="90" spans="1:2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -8506,7 +8113,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="91" ht="15.75" spans="1:2">
+    <row r="91" spans="1:2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -8514,7 +8121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="92" ht="15.75" spans="1:2">
+    <row r="92" spans="1:2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -8522,7 +8129,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="93" ht="15.75" spans="1:2">
+    <row r="93" spans="1:2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -8530,7 +8137,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" ht="15.75" spans="1:2">
+    <row r="94" spans="1:2">
       <c r="A94">
         <v>2</v>
       </c>
@@ -8538,7 +8145,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="95" ht="15.75" spans="1:2">
+    <row r="95" spans="1:2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -8546,7 +8153,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="96" ht="15.75" spans="1:2">
+    <row r="96" spans="1:2">
       <c r="A96">
         <v>2</v>
       </c>
@@ -8554,7 +8161,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" ht="15.75" spans="1:2">
+    <row r="97" spans="1:2">
       <c r="A97">
         <v>2</v>
       </c>
@@ -8562,7 +8169,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="98" ht="15.75" spans="1:2">
+    <row r="98" spans="1:2">
       <c r="A98">
         <v>1</v>
       </c>
@@ -8570,7 +8177,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="99" ht="15.75" spans="1:2">
+    <row r="99" spans="1:2">
       <c r="A99">
         <v>1</v>
       </c>
@@ -8578,7 +8185,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="100" ht="15.75" spans="1:2">
+    <row r="100" spans="1:2">
       <c r="A100">
         <v>0</v>
       </c>
@@ -8586,7 +8193,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="101" ht="15.75" spans="1:2">
+    <row r="101" spans="1:2">
       <c r="A101">
         <v>0</v>
       </c>
@@ -8594,7 +8201,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="102" ht="15.75" spans="1:2">
+    <row r="102" spans="1:2">
       <c r="A102">
         <v>0</v>
       </c>
@@ -8602,7 +8209,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="103" ht="15.75" spans="1:2">
+    <row r="103" spans="1:2">
       <c r="A103">
         <v>1</v>
       </c>
@@ -8610,7 +8217,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="104" ht="15.75" spans="1:2">
+    <row r="104" spans="1:2">
       <c r="A104">
         <v>1</v>
       </c>
@@ -8618,7 +8225,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" ht="15.75" spans="1:2">
+    <row r="105" spans="1:2">
       <c r="A105">
         <v>1</v>
       </c>
@@ -8626,7 +8233,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" ht="15.75" spans="1:2">
+    <row r="106" spans="1:2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -8634,7 +8241,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" ht="15.75" spans="1:2">
+    <row r="107" spans="1:2">
       <c r="A107">
         <v>1</v>
       </c>
@@ -8642,7 +8249,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="108" ht="15.75" spans="1:2">
+    <row r="108" spans="1:2">
       <c r="A108">
         <v>1</v>
       </c>
@@ -8650,7 +8257,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="109" ht="15.75" spans="1:2">
+    <row r="109" spans="1:2">
       <c r="A109">
         <v>0</v>
       </c>
@@ -8658,7 +8265,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="110" ht="15.75" spans="1:2">
+    <row r="110" spans="1:2">
       <c r="A110">
         <v>2</v>
       </c>
@@ -8666,7 +8273,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="111" ht="15.75" spans="1:2">
+    <row r="111" spans="1:2">
       <c r="A111">
         <v>1</v>
       </c>
@@ -8674,7 +8281,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="112" ht="15.75" spans="1:2">
+    <row r="112" spans="1:2">
       <c r="A112">
         <v>1</v>
       </c>
@@ -8682,7 +8289,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="113" ht="15.75" spans="1:2">
+    <row r="113" spans="1:2">
       <c r="A113">
         <v>1</v>
       </c>
@@ -8690,7 +8297,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="114" ht="15.75" spans="1:2">
+    <row r="114" spans="1:2">
       <c r="A114">
         <v>2</v>
       </c>
@@ -8698,7 +8305,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" ht="15.75" spans="1:2">
+    <row r="115" spans="1:2">
       <c r="A115">
         <v>0</v>
       </c>
@@ -8706,7 +8313,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="116" ht="15.75" spans="1:2">
+    <row r="116" spans="1:2">
       <c r="A116">
         <v>1</v>
       </c>
@@ -8714,7 +8321,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="117" ht="15.75" spans="1:2">
+    <row r="117" spans="1:2">
       <c r="A117">
         <v>0</v>
       </c>
@@ -8722,7 +8329,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="118" ht="15.75" spans="1:2">
+    <row r="118" spans="1:2">
       <c r="A118">
         <v>0</v>
       </c>
@@ -8730,7 +8337,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="119" ht="15.75" spans="1:2">
+    <row r="119" spans="1:2">
       <c r="A119">
         <v>0</v>
       </c>
@@ -8738,7 +8345,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="120" ht="15.75" spans="1:2">
+    <row r="120" spans="1:2">
       <c r="A120">
         <v>0</v>
       </c>
@@ -8746,7 +8353,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="121" ht="15.75" spans="1:2">
+    <row r="121" spans="1:2">
       <c r="A121">
         <v>0</v>
       </c>
@@ -8754,7 +8361,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="122" ht="15.75" spans="1:2">
+    <row r="122" spans="1:2">
       <c r="A122">
         <v>1</v>
       </c>
@@ -8762,7 +8369,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="123" ht="15.75" spans="1:2">
+    <row r="123" spans="1:2">
       <c r="A123">
         <v>1</v>
       </c>
@@ -8770,7 +8377,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="124" ht="15.75" spans="1:2">
+    <row r="124" spans="1:2">
       <c r="A124">
         <v>1</v>
       </c>
@@ -8778,7 +8385,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="125" ht="15.75" spans="1:2">
+    <row r="125" spans="1:2">
       <c r="A125">
         <v>2</v>
       </c>
@@ -8786,7 +8393,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="126" ht="15.75" spans="1:2">
+    <row r="126" spans="1:2">
       <c r="A126">
         <v>0</v>
       </c>
@@ -8794,7 +8401,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="127" ht="15.75" spans="1:2">
+    <row r="127" spans="1:2">
       <c r="A127">
         <v>1</v>
       </c>
@@ -8802,7 +8409,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="128" ht="15.75" spans="1:2">
+    <row r="128" spans="1:2">
       <c r="A128">
         <v>1</v>
       </c>
@@ -8810,7 +8417,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="129" ht="15.75" spans="1:2">
+    <row r="129" spans="1:2">
       <c r="A129">
         <v>2</v>
       </c>
@@ -8818,7 +8425,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="130" ht="15.75" spans="1:2">
+    <row r="130" spans="1:2">
       <c r="A130">
         <v>1</v>
       </c>
@@ -8826,7 +8433,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="131" ht="15.75" spans="1:2">
+    <row r="131" spans="1:2">
       <c r="A131">
         <v>1</v>
       </c>
@@ -8834,7 +8441,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="132" ht="15.75" spans="1:2">
+    <row r="132" spans="1:2">
       <c r="A132">
         <v>1</v>
       </c>
@@ -8842,7 +8449,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="133" ht="15.75" spans="1:2">
+    <row r="133" spans="1:2">
       <c r="A133">
         <v>1</v>
       </c>
@@ -8850,7 +8457,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="134" ht="15.75" spans="1:2">
+    <row r="134" spans="1:2">
       <c r="A134">
         <v>1</v>
       </c>
@@ -8858,7 +8465,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="135" ht="15.75" spans="1:2">
+    <row r="135" spans="1:2">
       <c r="A135">
         <v>1</v>
       </c>
@@ -8866,7 +8473,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="136" ht="15.75" spans="1:2">
+    <row r="136" spans="1:2">
       <c r="A136">
         <v>1</v>
       </c>
@@ -8874,7 +8481,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="137" ht="15.75" spans="1:2">
+    <row r="137" spans="1:2">
       <c r="A137">
         <v>1</v>
       </c>
@@ -8882,7 +8489,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="138" ht="15.75" spans="1:2">
+    <row r="138" spans="1:2">
       <c r="A138">
         <v>2</v>
       </c>
@@ -8890,7 +8497,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="139" ht="15.75" spans="1:2">
+    <row r="139" spans="1:2">
       <c r="A139">
         <v>2</v>
       </c>
@@ -8898,7 +8505,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="140" ht="15.75" spans="1:2">
+    <row r="140" spans="1:2">
       <c r="A140">
         <v>0</v>
       </c>
@@ -8906,7 +8513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="141" ht="15.75" spans="1:2">
+    <row r="141" spans="1:2">
       <c r="A141">
         <v>2</v>
       </c>
@@ -8914,7 +8521,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="142" ht="15.75" spans="1:2">
+    <row r="142" spans="1:2">
       <c r="A142">
         <v>2</v>
       </c>
@@ -8922,7 +8529,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="143" ht="15.75" spans="1:2">
+    <row r="143" spans="1:2">
       <c r="A143">
         <v>2</v>
       </c>
@@ -8930,7 +8537,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="144" ht="15.75" spans="1:2">
+    <row r="144" spans="1:2">
       <c r="A144">
         <v>2</v>
       </c>
@@ -8938,7 +8545,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="145" ht="15.75" spans="1:2">
+    <row r="145" spans="1:2">
       <c r="A145">
         <v>2</v>
       </c>
@@ -8946,7 +8553,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="146" ht="15.75" spans="1:2">
+    <row r="146" spans="1:2">
       <c r="A146">
         <v>1</v>
       </c>
@@ -8954,7 +8561,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="147" ht="15.75" spans="1:2">
+    <row r="147" spans="1:2">
       <c r="A147">
         <v>2</v>
       </c>
@@ -8962,7 +8569,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="148" ht="15.75" spans="1:2">
+    <row r="148" spans="1:2">
       <c r="A148">
         <v>2</v>
       </c>
@@ -8970,7 +8577,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="149" ht="15.75" spans="1:2">
+    <row r="149" spans="1:2">
       <c r="A149">
         <v>2</v>
       </c>
@@ -8978,7 +8585,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="150" ht="15.75" spans="1:2">
+    <row r="150" spans="1:2">
       <c r="A150">
         <v>2</v>
       </c>
@@ -8986,7 +8593,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="151" ht="15.75" spans="1:2">
+    <row r="151" spans="1:2">
       <c r="A151">
         <v>2</v>
       </c>
@@ -8994,7 +8601,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="152" ht="15.75" spans="1:2">
+    <row r="152" spans="1:2">
       <c r="A152">
         <v>0</v>
       </c>
@@ -9002,7 +8609,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="153" ht="15.75" spans="1:2">
+    <row r="153" spans="1:2">
       <c r="A153">
         <v>1</v>
       </c>
@@ -9010,7 +8617,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="154" ht="15.75" spans="1:2">
+    <row r="154" spans="1:2">
       <c r="A154">
         <v>0</v>
       </c>
@@ -9018,7 +8625,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="155" ht="15.75" spans="1:2">
+    <row r="155" spans="1:2">
       <c r="A155">
         <v>2</v>
       </c>
@@ -9026,7 +8633,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="156" ht="15.75" spans="1:2">
+    <row r="156" spans="1:2">
       <c r="A156">
         <v>2</v>
       </c>
@@ -9034,7 +8641,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="157" ht="15.75" spans="1:2">
+    <row r="157" spans="1:2">
       <c r="A157">
         <v>1</v>
       </c>
@@ -9042,7 +8649,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="158" ht="15.75" spans="1:2">
+    <row r="158" spans="1:2">
       <c r="A158">
         <v>1</v>
       </c>
@@ -9050,7 +8657,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="159" ht="15.75" spans="1:2">
+    <row r="159" spans="1:2">
       <c r="A159">
         <v>0</v>
       </c>
@@ -9058,7 +8665,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="160" ht="15.75" spans="1:2">
+    <row r="160" spans="1:2">
       <c r="A160">
         <v>0</v>
       </c>
@@ -9066,7 +8673,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="161" ht="15.75" spans="1:2">
+    <row r="161" spans="1:2">
       <c r="A161">
         <v>1</v>
       </c>
@@ -9074,7 +8681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="162" ht="15.75" spans="1:2">
+    <row r="162" spans="1:2">
       <c r="A162">
         <v>2</v>
       </c>
@@ -9082,7 +8689,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="163" ht="15.75" spans="1:2">
+    <row r="163" spans="1:2">
       <c r="A163">
         <v>0</v>
       </c>
@@ -9090,7 +8697,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="164" ht="15.75" spans="1:2">
+    <row r="164" spans="1:2">
       <c r="A164">
         <v>0</v>
       </c>
@@ -9098,7 +8705,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="165" ht="15.75" spans="1:2">
+    <row r="165" spans="1:2">
       <c r="A165">
         <v>0</v>
       </c>
@@ -9106,7 +8713,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="166" ht="15.75" spans="1:2">
+    <row r="166" spans="1:2">
       <c r="A166">
         <v>2</v>
       </c>
@@ -9114,7 +8721,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="167" ht="15.75" spans="1:2">
+    <row r="167" spans="1:2">
       <c r="A167">
         <v>0</v>
       </c>
@@ -9122,7 +8729,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="168" ht="15.75" spans="1:2">
+    <row r="168" spans="1:2">
       <c r="A168">
         <v>0</v>
       </c>
@@ -9130,7 +8737,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="169" ht="15.75" spans="1:2">
+    <row r="169" spans="1:2">
       <c r="A169">
         <v>0</v>
       </c>
@@ -9138,7 +8745,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="170" ht="15.75" spans="1:2">
+    <row r="170" spans="1:2">
       <c r="A170">
         <v>0</v>
       </c>
@@ -9146,7 +8753,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="171" ht="15.75" spans="1:2">
+    <row r="171" spans="1:2">
       <c r="A171">
         <v>0</v>
       </c>
@@ -9154,7 +8761,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="172" ht="15.75" spans="1:2">
+    <row r="172" spans="1:2">
       <c r="A172">
         <v>0</v>
       </c>
@@ -9162,7 +8769,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="173" ht="15.75" spans="1:2">
+    <row r="173" spans="1:2">
       <c r="A173">
         <v>0</v>
       </c>
@@ -9170,7 +8777,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="174" ht="15.75" spans="1:2">
+    <row r="174" spans="1:2">
       <c r="A174">
         <v>0</v>
       </c>
@@ -9178,7 +8785,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="175" ht="15.75" spans="1:2">
+    <row r="175" spans="1:2">
       <c r="A175">
         <v>1</v>
       </c>
@@ -9186,7 +8793,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="176" ht="15.75" spans="1:2">
+    <row r="176" spans="1:2">
       <c r="A176">
         <v>1</v>
       </c>
@@ -9194,7 +8801,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="177" ht="15.75" spans="1:2">
+    <row r="177" spans="1:2">
       <c r="A177">
         <v>1</v>
       </c>
@@ -9202,7 +8809,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="178" ht="15.75" spans="1:2">
+    <row r="178" spans="1:2">
       <c r="A178">
         <v>1</v>
       </c>
@@ -9210,7 +8817,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="179" ht="15.75" spans="1:2">
+    <row r="179" spans="1:2">
       <c r="A179">
         <v>1</v>
       </c>
@@ -9218,7 +8825,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="180" ht="15.75" spans="1:2">
+    <row r="180" spans="1:2">
       <c r="A180">
         <v>1</v>
       </c>
@@ -9226,7 +8833,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="181" ht="15.75" spans="1:2">
+    <row r="181" spans="1:2">
       <c r="A181">
         <v>1</v>
       </c>
@@ -9234,7 +8841,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="182" ht="15.75" spans="1:2">
+    <row r="182" spans="1:2">
       <c r="A182">
         <v>1</v>
       </c>
@@ -9242,7 +8849,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="183" ht="15.75" spans="1:2">
+    <row r="183" spans="1:2">
       <c r="A183">
         <v>1</v>
       </c>
@@ -9250,7 +8857,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="184" ht="15.75" spans="1:2">
+    <row r="184" spans="1:2">
       <c r="A184">
         <v>2</v>
       </c>
@@ -9258,7 +8865,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="185" ht="15.75" spans="1:2">
+    <row r="185" spans="1:2">
       <c r="A185">
         <v>1</v>
       </c>
@@ -9266,7 +8873,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="186" ht="15.75" spans="1:2">
+    <row r="186" spans="1:2">
       <c r="A186">
         <v>2</v>
       </c>
@@ -9274,7 +8881,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="187" ht="15.75" spans="1:2">
+    <row r="187" spans="1:2">
       <c r="A187">
         <v>1</v>
       </c>
@@ -9282,7 +8889,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="188" ht="15.75" spans="1:2">
+    <row r="188" spans="1:2">
       <c r="A188">
         <v>2</v>
       </c>
@@ -9290,7 +8897,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="189" ht="15.75" spans="1:2">
+    <row r="189" spans="1:2">
       <c r="A189">
         <v>1</v>
       </c>
@@ -9298,7 +8905,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="190" ht="15.75" spans="1:2">
+    <row r="190" spans="1:2">
       <c r="A190">
         <v>2</v>
       </c>
@@ -9306,7 +8913,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="191" ht="15.75" spans="1:2">
+    <row r="191" spans="1:2">
       <c r="A191">
         <v>1</v>
       </c>
@@ -9314,7 +8921,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="192" ht="15.75" spans="1:2">
+    <row r="192" spans="1:2">
       <c r="A192">
         <v>1</v>
       </c>
@@ -9322,7 +8929,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="193" ht="15.75" spans="1:2">
+    <row r="193" spans="1:2">
       <c r="A193">
         <v>0</v>
       </c>
@@ -9330,7 +8937,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="194" ht="15.75" spans="1:2">
+    <row r="194" spans="1:2">
       <c r="A194">
         <v>0</v>
       </c>
@@ -9338,7 +8945,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="195" ht="15.75" spans="1:2">
+    <row r="195" spans="1:2">
       <c r="A195">
         <v>0</v>
       </c>
@@ -9346,7 +8953,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="196" ht="15.75" spans="1:2">
+    <row r="196" spans="1:2">
       <c r="A196">
         <v>1</v>
       </c>
@@ -9354,7 +8961,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="197" ht="15.75" spans="1:2">
+    <row r="197" spans="1:2">
       <c r="A197">
         <v>1</v>
       </c>
@@ -9362,7 +8969,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="198" ht="15.75" spans="1:2">
+    <row r="198" spans="1:2">
       <c r="A198">
         <v>1</v>
       </c>
@@ -9370,7 +8977,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="199" ht="15.75" spans="1:2">
+    <row r="199" spans="1:2">
       <c r="A199">
         <v>2</v>
       </c>
@@ -9378,7 +8985,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="200" ht="15.75" spans="1:2">
+    <row r="200" spans="1:2">
       <c r="A200">
         <v>1</v>
       </c>
@@ -9386,7 +8993,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="201" ht="15.75" spans="1:2">
+    <row r="201" spans="1:2">
       <c r="A201">
         <v>2</v>
       </c>
@@ -9394,7 +9001,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="202" ht="15.75" spans="1:2">
+    <row r="202" spans="1:2">
       <c r="A202">
         <v>2</v>
       </c>
@@ -9402,7 +9009,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="203" ht="15.75" spans="1:2">
+    <row r="203" spans="1:2">
       <c r="A203">
         <v>1</v>
       </c>
@@ -9410,7 +9017,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="204" ht="15.75" spans="1:2">
+    <row r="204" spans="1:2">
       <c r="A204">
         <v>1</v>
       </c>
@@ -9418,7 +9025,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="205" ht="15.75" spans="1:2">
+    <row r="205" spans="1:2">
       <c r="A205">
         <v>1</v>
       </c>
@@ -9426,7 +9033,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="206" ht="15.75" spans="1:2">
+    <row r="206" spans="1:2">
       <c r="A206">
         <v>1</v>
       </c>
@@ -9434,7 +9041,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="207" ht="15.75" spans="1:2">
+    <row r="207" spans="1:2">
       <c r="A207">
         <v>1</v>
       </c>
@@ -9442,7 +9049,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="208" ht="15.75" spans="1:2">
+    <row r="208" spans="1:2">
       <c r="A208">
         <v>0</v>
       </c>
@@ -9450,7 +9057,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="209" ht="15.75" spans="1:2">
+    <row r="209" spans="1:2">
       <c r="A209">
         <v>0</v>
       </c>
@@ -9458,7 +9065,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="210" ht="15.75" spans="1:2">
+    <row r="210" spans="1:2">
       <c r="A210">
         <v>2</v>
       </c>
@@ -9466,7 +9073,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="211" ht="15.75" spans="1:2">
+    <row r="211" spans="1:2">
       <c r="A211">
         <v>2</v>
       </c>
@@ -9474,7 +9081,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="212" ht="15.75" spans="1:2">
+    <row r="212" spans="1:2">
       <c r="A212">
         <v>1</v>
       </c>
@@ -9482,7 +9089,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="213" ht="15.75" spans="1:2">
+    <row r="213" spans="1:2">
       <c r="A213">
         <v>1</v>
       </c>
@@ -9490,7 +9097,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="214" ht="15.75" spans="1:2">
+    <row r="214" spans="1:2">
       <c r="A214">
         <v>1</v>
       </c>
@@ -9498,7 +9105,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="215" ht="15.75" spans="1:2">
+    <row r="215" spans="1:2">
       <c r="A215">
         <v>1</v>
       </c>
@@ -9506,7 +9113,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="216" ht="15.75" spans="1:2">
+    <row r="216" spans="1:2">
       <c r="A216">
         <v>1</v>
       </c>
@@ -9514,7 +9121,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="217" ht="15.75" spans="1:2">
+    <row r="217" spans="1:2">
       <c r="A217">
         <v>1</v>
       </c>
@@ -9522,7 +9129,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="218" ht="15.75" spans="1:2">
+    <row r="218" spans="1:2">
       <c r="A218">
         <v>2</v>
       </c>
@@ -9530,7 +9137,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="219" ht="15.75" spans="1:2">
+    <row r="219" spans="1:2">
       <c r="A219">
         <v>0</v>
       </c>
@@ -9538,7 +9145,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="220" ht="15.75" spans="1:2">
+    <row r="220" spans="1:2">
       <c r="A220">
         <v>2</v>
       </c>
@@ -9546,7 +9153,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="221" ht="15.75" spans="1:2">
+    <row r="221" spans="1:2">
       <c r="A221">
         <v>1</v>
       </c>
@@ -9554,7 +9161,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="222" ht="15.75" spans="1:2">
+    <row r="222" spans="1:2">
       <c r="A222">
         <v>1</v>
       </c>
@@ -9562,7 +9169,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="223" ht="15.75" spans="1:2">
+    <row r="223" spans="1:2">
       <c r="A223">
         <v>1</v>
       </c>
@@ -9570,7 +9177,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="224" ht="15.75" spans="1:2">
+    <row r="224" spans="1:2">
       <c r="A224">
         <v>1</v>
       </c>
@@ -9578,7 +9185,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="225" ht="15.75" spans="1:2">
+    <row r="225" spans="1:2">
       <c r="A225">
         <v>1</v>
       </c>
@@ -9586,7 +9193,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="226" ht="15.75" spans="1:2">
+    <row r="226" spans="1:2">
       <c r="A226">
         <v>2</v>
       </c>
@@ -9594,7 +9201,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="227" ht="15.75" spans="1:2">
+    <row r="227" spans="1:2">
       <c r="A227">
         <v>1</v>
       </c>
@@ -9602,7 +9209,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="228" ht="15.75" spans="1:2">
+    <row r="228" spans="1:2">
       <c r="A228">
         <v>1</v>
       </c>
@@ -9610,7 +9217,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="229" ht="15.75" spans="1:2">
+    <row r="229" spans="1:2">
       <c r="A229">
         <v>1</v>
       </c>
@@ -9618,7 +9225,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="230" ht="15.75" spans="1:2">
+    <row r="230" spans="1:2">
       <c r="A230">
         <v>0</v>
       </c>
@@ -9626,7 +9233,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="231" ht="15.75" spans="1:2">
+    <row r="231" spans="1:2">
       <c r="A231">
         <v>1</v>
       </c>
@@ -9634,7 +9241,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="232" ht="15.75" spans="1:2">
+    <row r="232" spans="1:2">
       <c r="A232">
         <v>1</v>
       </c>
@@ -9642,7 +9249,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="233" ht="15.75" spans="1:2">
+    <row r="233" spans="1:2">
       <c r="A233">
         <v>1</v>
       </c>
@@ -9650,7 +9257,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="234" ht="15.75" spans="1:2">
+    <row r="234" spans="1:2">
       <c r="A234">
         <v>1</v>
       </c>
@@ -9658,7 +9265,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="235" ht="15.75" spans="1:2">
+    <row r="235" spans="1:2">
       <c r="A235">
         <v>2</v>
       </c>
@@ -9666,7 +9273,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="236" ht="15.75" spans="1:2">
+    <row r="236" spans="1:2">
       <c r="A236">
         <v>2</v>
       </c>
@@ -9674,7 +9281,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="237" ht="15.75" spans="1:2">
+    <row r="237" spans="1:2">
       <c r="A237">
         <v>1</v>
       </c>
@@ -9682,7 +9289,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="238" ht="15.75" spans="1:2">
+    <row r="238" spans="1:2">
       <c r="A238">
         <v>1</v>
       </c>
@@ -9690,7 +9297,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="239" ht="15.75" spans="1:2">
+    <row r="239" spans="1:2">
       <c r="A239">
         <v>0</v>
       </c>
@@ -9698,7 +9305,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="240" ht="15.75" spans="1:2">
+    <row r="240" spans="1:2">
       <c r="A240">
         <v>1</v>
       </c>
@@ -9706,7 +9313,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="241" ht="15.75" spans="1:2">
+    <row r="241" spans="1:2">
       <c r="A241">
         <v>1</v>
       </c>
@@ -9714,7 +9321,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="242" ht="15.75" spans="1:2">
+    <row r="242" spans="1:2">
       <c r="A242">
         <v>2</v>
       </c>
@@ -9722,7 +9329,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="243" ht="15.75" spans="1:2">
+    <row r="243" spans="1:2">
       <c r="A243">
         <v>1</v>
       </c>
@@ -9730,7 +9337,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="244" ht="15.75" spans="1:2">
+    <row r="244" spans="1:2">
       <c r="A244">
         <v>0</v>
       </c>
@@ -9738,7 +9345,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="245" ht="15.75" spans="1:2">
+    <row r="245" spans="1:2">
       <c r="A245">
         <v>0</v>
       </c>
@@ -9746,7 +9353,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="246" ht="15.75" spans="1:2">
+    <row r="246" spans="1:2">
       <c r="A246">
         <v>1</v>
       </c>
@@ -9754,7 +9361,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="247" ht="15.75" spans="1:2">
+    <row r="247" spans="1:2">
       <c r="A247">
         <v>2</v>
       </c>
@@ -9762,7 +9369,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="248" ht="15.75" spans="1:2">
+    <row r="248" spans="1:2">
       <c r="A248">
         <v>0</v>
       </c>
@@ -9770,7 +9377,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="249" ht="15.75" spans="1:2">
+    <row r="249" spans="1:2">
       <c r="A249">
         <v>0</v>
       </c>
@@ -9778,7 +9385,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="250" ht="15.75" spans="1:2">
+    <row r="250" spans="1:2">
       <c r="A250">
         <v>0</v>
       </c>
@@ -9786,7 +9393,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="251" ht="15.75" spans="1:2">
+    <row r="251" spans="1:2">
       <c r="A251">
         <v>0</v>
       </c>
@@ -9794,7 +9401,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="252" ht="15.75" spans="1:2">
+    <row r="252" spans="1:2">
       <c r="A252">
         <v>0</v>
       </c>
@@ -9802,7 +9409,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="253" ht="15.75" spans="1:2">
+    <row r="253" spans="1:2">
       <c r="A253">
         <v>1</v>
       </c>
@@ -9810,7 +9417,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="254" ht="15.75" spans="1:2">
+    <row r="254" spans="1:2">
       <c r="A254">
         <v>2</v>
       </c>
@@ -9818,7 +9425,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="255" ht="15.75" spans="1:2">
+    <row r="255" spans="1:2">
       <c r="A255">
         <v>2</v>
       </c>
@@ -9826,7 +9433,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="256" ht="15.75" spans="1:2">
+    <row r="256" spans="1:2">
       <c r="A256">
         <v>1</v>
       </c>
@@ -9834,7 +9441,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="257" ht="15.75" spans="1:2">
+    <row r="257" spans="1:2">
       <c r="A257">
         <v>2</v>
       </c>
@@ -9842,7 +9449,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="258" ht="15.75" spans="1:2">
+    <row r="258" spans="1:2">
       <c r="A258">
         <v>1</v>
       </c>
@@ -9850,7 +9457,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="259" ht="15.75" spans="1:2">
+    <row r="259" spans="1:2">
       <c r="A259">
         <v>1</v>
       </c>
@@ -9858,7 +9465,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="260" ht="15.75" spans="1:2">
+    <row r="260" spans="1:2">
       <c r="A260">
         <v>2</v>
       </c>
@@ -9866,7 +9473,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="261" ht="15.75" spans="1:2">
+    <row r="261" spans="1:2">
       <c r="A261">
         <v>2</v>
       </c>
@@ -9874,7 +9481,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="262" ht="15.75" spans="1:2">
+    <row r="262" spans="1:2">
       <c r="A262">
         <v>0</v>
       </c>
@@ -9882,7 +9489,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="263" ht="15.75" spans="1:2">
+    <row r="263" spans="1:2">
       <c r="A263">
         <v>1</v>
       </c>
@@ -9890,7 +9497,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="264" ht="15.75" spans="1:2">
+    <row r="264" spans="1:2">
       <c r="A264">
         <v>2</v>
       </c>
@@ -9898,7 +9505,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="265" ht="15.75" spans="1:2">
+    <row r="265" spans="1:2">
       <c r="A265">
         <v>1</v>
       </c>
@@ -9906,7 +9513,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="266" ht="15.75" spans="1:2">
+    <row r="266" spans="1:2">
       <c r="A266">
         <v>2</v>
       </c>
@@ -9914,7 +9521,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="267" ht="15.75" spans="1:2">
+    <row r="267" spans="1:2">
       <c r="A267">
         <v>2</v>
       </c>
@@ -9922,7 +9529,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="268" ht="15.75" spans="1:2">
+    <row r="268" spans="1:2">
       <c r="A268">
         <v>1</v>
       </c>
@@ -9930,7 +9537,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="269" ht="15.75" spans="1:2">
+    <row r="269" spans="1:2">
       <c r="A269">
         <v>1</v>
       </c>
@@ -9970,7 +9577,7 @@
         <v>7217242</v>
       </c>
     </row>
-    <row r="274" ht="120" spans="1:2">
+    <row r="274" spans="1:2" ht="120">
       <c r="A274">
         <v>2</v>
       </c>
@@ -10394,7 +10001,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="327" ht="195" spans="1:2">
+    <row r="327" spans="1:2" ht="195">
       <c r="A327">
         <v>2</v>
       </c>
@@ -10562,7 +10169,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="348" ht="30" spans="1:2">
+    <row r="348" spans="1:2" ht="30">
       <c r="A348">
         <v>0</v>
       </c>
@@ -10826,7 +10433,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="381" ht="45" spans="1:2">
+    <row r="381" spans="1:2" ht="45">
       <c r="A381">
         <v>2</v>
       </c>
@@ -11018,7 +10625,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="405" ht="75" spans="1:2">
+    <row r="405" spans="1:2" ht="75">
       <c r="A405">
         <v>2</v>
       </c>
@@ -11082,7 +10689,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="413" ht="165" spans="1:2">
+    <row r="413" spans="1:2" ht="165">
       <c r="A413">
         <v>2</v>
       </c>
@@ -11242,7 +10849,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="433" ht="30" spans="1:2">
+    <row r="433" spans="1:2" ht="30">
       <c r="A433">
         <v>2</v>
       </c>
@@ -11258,7 +10865,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="435" ht="90" spans="1:2">
+    <row r="435" spans="1:2" ht="90">
       <c r="A435">
         <v>2</v>
       </c>
@@ -11378,7 +10985,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="450" ht="60" spans="1:2">
+    <row r="450" spans="1:2" ht="60">
       <c r="A450">
         <v>2</v>
       </c>
@@ -11562,7 +11169,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="473" ht="75" spans="1:2">
+    <row r="473" spans="1:2" ht="75">
       <c r="A473">
         <v>0</v>
       </c>
@@ -11634,7 +11241,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="482" ht="75" spans="1:2">
+    <row r="482" spans="1:2" ht="75">
       <c r="A482">
         <v>0</v>
       </c>
@@ -11650,7 +11257,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="484" ht="75" spans="1:2">
+    <row r="484" spans="1:2" ht="75">
       <c r="A484">
         <v>0</v>
       </c>
@@ -11666,7 +11273,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="486" ht="75" spans="1:2">
+    <row r="486" spans="1:2" ht="75">
       <c r="A486">
         <v>0</v>
       </c>
@@ -11714,7 +11321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="492" ht="150" spans="1:2">
+    <row r="492" spans="1:2" ht="150">
       <c r="A492">
         <v>2</v>
       </c>
@@ -11802,7 +11409,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="503" ht="75" spans="1:2">
+    <row r="503" spans="1:2" ht="75">
       <c r="A503">
         <v>0</v>
       </c>
@@ -12018,7 +11625,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="530" ht="90" spans="1:2">
+    <row r="530" spans="1:2" ht="90">
       <c r="A530">
         <v>2</v>
       </c>
@@ -12122,7 +11729,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="543" ht="75" spans="1:2">
+    <row r="543" spans="1:2" ht="75">
       <c r="A543">
         <v>2</v>
       </c>
@@ -12170,7 +11777,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="549" ht="135" spans="1:2">
+    <row r="549" spans="1:2" ht="135">
       <c r="A549">
         <v>2</v>
       </c>
@@ -12178,7 +11785,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="550" ht="75" spans="1:2">
+    <row r="550" spans="1:2" ht="75">
       <c r="A550">
         <v>2</v>
       </c>
@@ -12306,7 +11913,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="566" ht="90" spans="1:2">
+    <row r="566" spans="1:2" ht="90">
       <c r="A566">
         <v>2</v>
       </c>
@@ -12330,7 +11937,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="569" ht="120" spans="1:2">
+    <row r="569" spans="1:2" ht="120">
       <c r="A569">
         <v>2</v>
       </c>
@@ -12466,7 +12073,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="586" ht="30" spans="1:2">
+    <row r="586" spans="1:2" ht="30">
       <c r="A586">
         <v>0</v>
       </c>
@@ -12490,7 +12097,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="589" ht="60" spans="1:2">
+    <row r="589" spans="1:2" ht="60">
       <c r="A589">
         <v>0</v>
       </c>
@@ -12530,7 +12137,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="594" ht="30" spans="1:2">
+    <row r="594" spans="1:2" ht="30">
       <c r="A594">
         <v>0</v>
       </c>
@@ -12722,7 +12329,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="618" ht="75" spans="1:2">
+    <row r="618" spans="1:2" ht="75">
       <c r="A618">
         <v>2</v>
       </c>
@@ -12754,7 +12361,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="622" ht="90" spans="1:2">
+    <row r="622" spans="1:2" ht="90">
       <c r="A622">
         <v>2</v>
       </c>
@@ -13178,7 +12785,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="675" ht="120" spans="1:2">
+    <row r="675" spans="1:2" ht="120">
       <c r="A675">
         <v>0</v>
       </c>
@@ -13314,7 +12921,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="692" ht="75" spans="1:2">
+    <row r="692" spans="1:2" ht="75">
       <c r="A692">
         <v>0</v>
       </c>
@@ -13378,7 +12985,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="700" ht="75" spans="1:2">
+    <row r="700" spans="1:2" ht="75">
       <c r="A700">
         <v>2</v>
       </c>
@@ -13498,7 +13105,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="715" ht="135" spans="1:2">
+    <row r="715" spans="1:2" ht="135">
       <c r="A715">
         <v>2</v>
       </c>
@@ -13554,7 +13161,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="722" ht="60" spans="1:2">
+    <row r="722" spans="1:2" ht="60">
       <c r="A722">
         <v>2</v>
       </c>
@@ -13562,7 +13169,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="723" ht="120" spans="1:2">
+    <row r="723" spans="1:2" ht="120">
       <c r="A723">
         <v>2</v>
       </c>
@@ -14266,7 +13873,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="811" ht="105" spans="1:2">
+    <row r="811" spans="1:2" ht="105">
       <c r="A811">
         <v>2</v>
       </c>
@@ -14282,7 +13889,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="813" ht="60" spans="1:2">
+    <row r="813" spans="1:2" ht="60">
       <c r="A813">
         <v>2</v>
       </c>
@@ -14298,7 +13905,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="815" ht="45" spans="1:2">
+    <row r="815" spans="1:2" ht="45">
       <c r="A815">
         <v>2</v>
       </c>
@@ -15010,7 +14617,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="904" ht="75" spans="1:2">
+    <row r="904" spans="1:2" ht="75">
       <c r="A904">
         <v>2</v>
       </c>
@@ -15034,7 +14641,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="907" ht="75" spans="1:2">
+    <row r="907" spans="1:2" ht="75">
       <c r="A907">
         <v>2</v>
       </c>
@@ -15058,7 +14665,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="910" ht="90" spans="1:2">
+    <row r="910" spans="1:2" ht="90">
       <c r="A910">
         <v>2</v>
       </c>
@@ -15106,7 +14713,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="916" ht="75" spans="1:2">
+    <row r="916" spans="1:2" ht="75">
       <c r="A916">
         <v>0</v>
       </c>
@@ -15114,7 +14721,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="917" ht="75" spans="1:2">
+    <row r="917" spans="1:2" ht="75">
       <c r="A917">
         <v>0</v>
       </c>
@@ -15196,7 +14803,7 @@
     </row>
     <row r="927" spans="1:2">
       <c r="A927">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B927" s="3" t="s">
         <v>736</v>
@@ -15204,7 +14811,7 @@
     </row>
     <row r="928" spans="1:2">
       <c r="A928">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B928" s="3" t="s">
         <v>736</v>
@@ -15220,7 +14827,7 @@
     </row>
     <row r="930" spans="1:2">
       <c r="A930">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B930" s="3" t="s">
         <v>736</v>
@@ -15252,7 +14859,7 @@
     </row>
     <row r="934" spans="1:2">
       <c r="A934">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B934" s="3" t="s">
         <v>702</v>
@@ -15276,7 +14883,7 @@
     </row>
     <row r="937" spans="1:2">
       <c r="A937">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B937" s="3" t="s">
         <v>741</v>
@@ -15420,7 +15027,7 @@
     </row>
     <row r="955" spans="1:2">
       <c r="A955">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B955" s="3" t="s">
         <v>758</v>
@@ -15474,7 +15081,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="962" ht="30" spans="1:2">
+    <row r="962" spans="1:2" ht="30">
       <c r="A962">
         <v>0</v>
       </c>
@@ -15740,7 +15347,7 @@
     </row>
     <row r="995" spans="1:2">
       <c r="A995">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B995" s="3" t="s">
         <v>149</v>
@@ -15938,8 +15545,608 @@
         <v>802</v>
       </c>
     </row>
+    <row r="1020" spans="1:2">
+      <c r="A1020">
+        <v>2</v>
+      </c>
+      <c r="B1020" s="5" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:2">
+      <c r="A1021">
+        <v>2</v>
+      </c>
+      <c r="B1021" s="6" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:2">
+      <c r="A1022">
+        <v>2</v>
+      </c>
+      <c r="B1022" s="6" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:2">
+      <c r="A1023">
+        <v>2</v>
+      </c>
+      <c r="B1023" s="6" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:2">
+      <c r="A1024">
+        <v>2</v>
+      </c>
+      <c r="B1024" s="6" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:2">
+      <c r="A1025">
+        <v>2</v>
+      </c>
+      <c r="B1025" s="6" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:2">
+      <c r="A1026">
+        <v>2</v>
+      </c>
+      <c r="B1026" s="6" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:2">
+      <c r="A1027">
+        <v>2</v>
+      </c>
+      <c r="B1027" s="6" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:2">
+      <c r="A1028">
+        <v>2</v>
+      </c>
+      <c r="B1028" s="6" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:2">
+      <c r="A1029">
+        <v>2</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:2">
+      <c r="A1030">
+        <v>2</v>
+      </c>
+      <c r="B1030" s="5" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:2">
+      <c r="A1031">
+        <v>2</v>
+      </c>
+      <c r="B1031" s="6" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:2">
+      <c r="A1032">
+        <v>2</v>
+      </c>
+      <c r="B1032" s="6" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:2">
+      <c r="A1033">
+        <v>2</v>
+      </c>
+      <c r="B1033" s="6" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:2">
+      <c r="A1034">
+        <v>2</v>
+      </c>
+      <c r="B1034" s="6" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:2">
+      <c r="A1035">
+        <v>2</v>
+      </c>
+      <c r="B1035" s="6" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:2">
+      <c r="A1036">
+        <v>2</v>
+      </c>
+      <c r="B1036" s="6" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:2">
+      <c r="A1037">
+        <v>2</v>
+      </c>
+      <c r="B1037" s="6" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:2">
+      <c r="A1038">
+        <v>2</v>
+      </c>
+      <c r="B1038" s="6" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:2">
+      <c r="A1039">
+        <v>2</v>
+      </c>
+      <c r="B1039" s="6" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:2">
+      <c r="A1040">
+        <v>2</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:2">
+      <c r="A1041">
+        <v>2</v>
+      </c>
+      <c r="B1041" s="6" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:2">
+      <c r="A1042">
+        <v>2</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:2">
+      <c r="A1043">
+        <v>2</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:2">
+      <c r="A1044">
+        <v>2</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:2">
+      <c r="A1045">
+        <v>2</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:2">
+      <c r="A1046">
+        <v>0</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:2">
+      <c r="A1047">
+        <v>0</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:2">
+      <c r="A1048">
+        <v>0</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:2">
+      <c r="A1049">
+        <v>0</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:2">
+      <c r="A1050">
+        <v>0</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:2">
+      <c r="A1051">
+        <v>0</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:2">
+      <c r="A1052">
+        <v>0</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:2">
+      <c r="A1053">
+        <v>0</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:2">
+      <c r="A1054">
+        <v>0</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:2">
+      <c r="A1055">
+        <v>0</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:2">
+      <c r="A1056">
+        <v>0</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:2">
+      <c r="A1057">
+        <v>0</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:2">
+      <c r="A1058">
+        <v>0</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:2">
+      <c r="A1059">
+        <v>0</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:2">
+      <c r="A1060">
+        <v>0</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:2">
+      <c r="A1061">
+        <v>0</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:2">
+      <c r="A1062">
+        <v>0</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:2">
+      <c r="A1063">
+        <v>0</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:2">
+      <c r="A1064">
+        <v>0</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:2">
+      <c r="A1065">
+        <v>0</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:2">
+      <c r="A1066">
+        <v>0</v>
+      </c>
+      <c r="B1066" s="6" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:2">
+      <c r="A1067">
+        <v>0</v>
+      </c>
+      <c r="B1067" s="6" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:2">
+      <c r="A1068">
+        <v>0</v>
+      </c>
+      <c r="B1068" s="6" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:2">
+      <c r="A1069">
+        <v>0</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:2">
+      <c r="A1070">
+        <v>0</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:2">
+      <c r="A1071">
+        <v>0</v>
+      </c>
+      <c r="B1071" s="6" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:2">
+      <c r="A1072">
+        <v>0</v>
+      </c>
+      <c r="B1072" s="6" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:2">
+      <c r="A1073">
+        <v>0</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:2">
+      <c r="A1074">
+        <v>0</v>
+      </c>
+      <c r="B1074" s="6" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:2">
+      <c r="A1075">
+        <v>0</v>
+      </c>
+      <c r="B1075" s="6" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:2">
+      <c r="A1076">
+        <v>0</v>
+      </c>
+      <c r="B1076" s="6" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:2">
+      <c r="A1077">
+        <v>0</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:2">
+      <c r="A1078">
+        <v>0</v>
+      </c>
+      <c r="B1078" s="6" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:2">
+      <c r="A1079">
+        <v>0</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:2">
+      <c r="A1080">
+        <v>0</v>
+      </c>
+      <c r="B1080" s="6" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:2">
+      <c r="A1081">
+        <v>0</v>
+      </c>
+      <c r="B1081" s="6" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:2">
+      <c r="A1082">
+        <v>0</v>
+      </c>
+      <c r="B1082" s="6" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:2">
+      <c r="A1083">
+        <v>0</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:2">
+      <c r="A1084">
+        <v>0</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:2">
+      <c r="A1085">
+        <v>0</v>
+      </c>
+      <c r="B1085" s="6" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:2">
+      <c r="A1086">
+        <v>0</v>
+      </c>
+      <c r="B1086" s="6" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:2">
+      <c r="A1087">
+        <v>0</v>
+      </c>
+      <c r="B1087" s="6" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:2">
+      <c r="A1088">
+        <v>0</v>
+      </c>
+      <c r="B1088" s="6" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:2">
+      <c r="A1089">
+        <v>0</v>
+      </c>
+      <c r="B1089" s="6" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:2">
+      <c r="A1090">
+        <v>0</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:2">
+      <c r="A1091">
+        <v>2</v>
+      </c>
+      <c r="B1091" s="6" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:2">
+      <c r="A1092">
+        <v>2</v>
+      </c>
+      <c r="B1092" s="6" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:2">
+      <c r="A1093">
+        <v>2</v>
+      </c>
+      <c r="B1093" s="6" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2">
+      <c r="A1094">
+        <v>2</v>
+      </c>
+      <c r="B1094" s="6" t="s">
+        <v>875</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>